<commit_message>
completed the testing matrix
</commit_message>
<xml_diff>
--- a/TestingMatrix.xlsx
+++ b/TestingMatrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\FinalProjectOOP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{268B4568-CF07-400C-A90C-6D5F76B8B8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4752B9-7251-45AF-A11E-526EA0277AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{291FF68A-396F-47C5-AAB0-B31113D1D0F2}"/>
   </bookViews>
@@ -36,24 +36,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Functioneaza citirea din fisiere?</t>
   </si>
   <si>
-    <t>Functioneaza functia execute din clasa CalculusStep?</t>
-  </si>
-  <si>
-    <t>Functioneaza functia addOperand din clasa CalculusStep?</t>
-  </si>
-  <si>
     <t>Se poate da skip unui pas?</t>
   </si>
   <si>
     <t>Daca apasam enter, trecem la urmatorul pas?</t>
   </si>
   <si>
-    <t>Functia userInteraction din clasa TextStep functioneaza?</t>
+    <t>Functia userInteraction functioneaza?</t>
+  </si>
+  <si>
+    <t>Functioneaza calcularea de screen skips?</t>
+  </si>
+  <si>
+    <t>Functioneaza calcularea error screen?</t>
+  </si>
+  <si>
+    <t>Functioneaza functia deleteFlow?</t>
+  </si>
+  <si>
+    <t>Functioneaza functia runFlow?</t>
+  </si>
+  <si>
+    <t>Putem oferi un nume flow-ului?</t>
+  </si>
+  <si>
+    <t>Putem oferi de la tastatura detalii legate de flow?</t>
+  </si>
+  <si>
+    <t>Putem alege tipul de step pe care dorim sa-l executam?</t>
+  </si>
+  <si>
+    <t>Putem alege tipul de operatie pe care vrem sa-l executam in Calculus Step?</t>
+  </si>
+  <si>
+    <t>Pot alege orice alta litera in afara de n pentru a continua?</t>
+  </si>
+  <si>
+    <t>Functia getTypeStep returneaza numele step-ului pe care eu il vrem?</t>
+  </si>
+  <si>
+    <t>La final flow-ul este considerat complet?</t>
+  </si>
+  <si>
+    <t>Putem oferi valori pentru fiecare parametru al fiecarui step?</t>
+  </si>
+  <si>
+    <t>Daca tipul de step ales este Output, primim informatii de la celelalte step-uri executate?</t>
+  </si>
+  <si>
+    <t>La final primim informatii despre ce step-uri am completat in timpul rularii flow-ului?</t>
+  </si>
+  <si>
+    <t>Atunci cand rularea flow-ului se incheie, putem afla momentul in care a fost creat flow-ul?</t>
+  </si>
+  <si>
+    <t>Putem oferi o descriere pentru un flow?</t>
   </si>
 </sst>
 </file>
@@ -406,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C16986-79A9-4E5B-B0B3-76E8C0D698B6}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,27 +466,97 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added functionality to write the informations that i give about a step in a certain file
</commit_message>
<xml_diff>
--- a/TestingMatrix.xlsx
+++ b/TestingMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\FinalProjectOOP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4752B9-7251-45AF-A11E-526EA0277AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C14D5DA-2645-4579-9F67-422C58CD31D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{291FF68A-396F-47C5-AAB0-B31113D1D0F2}"/>
   </bookViews>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>Functioneaza citirea din fisiere?</t>
-  </si>
-  <si>
     <t>Se poate da skip unui pas?</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Putem oferi o descriere pentru un flow?</t>
+  </si>
+  <si>
+    <t>Programul poate scrie la rulare informatiile pe care user-ul i le ofera intr-un fisier csv sau txt?</t>
   </si>
 </sst>
 </file>
@@ -450,9 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C16986-79A9-4E5B-B0B3-76E8C0D698B6}">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -461,102 +459,102 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>